<commit_message>
update filtering tempat kejadian
</commit_message>
<xml_diff>
--- a/hasil_clustering_gabungan.xlsx
+++ b/hasil_clustering_gabungan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\agis\agisni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F804BC81-AE34-4AD2-AE01-069D6DD1EE8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC374EE-ABE8-4056-AC67-D09823A52D95}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cluster_Umum" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="46">
   <si>
     <t>nama_kabupaten_kota</t>
   </si>
@@ -154,9 +154,6 @@
   </si>
   <si>
     <t>Tempat Kerja</t>
-  </si>
-  <si>
-    <t>cluster1</t>
   </si>
   <si>
     <t>latitude</t>
@@ -545,23 +542,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -587,13 +584,13 @@
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -625,7 +622,7 @@
         <v>107528627</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -657,7 +654,7 @@
         <v>107512302</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -689,7 +686,7 @@
         <v>107172509</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -721,7 +718,7 @@
         <v>106824965</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -753,7 +750,7 @@
         <v>1083514</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -785,7 +782,7 @@
         <v>107139542</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -817,7 +814,7 @@
         <v>108478858</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -849,7 +846,7 @@
         <v>107885592</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -881,7 +878,7 @@
         <v>108322903</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -913,7 +910,7 @@
         <v>10730529</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -945,7 +942,7 @@
         <v>108482982</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -977,7 +974,7 @@
         <v>108227876</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1009,7 +1006,7 @@
         <v>108495155</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1041,7 +1038,7 @@
         <v>107446541</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1073,7 +1070,7 @@
         <v>107762495</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1105,7 +1102,7 @@
         <v>106932576</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1137,7 +1134,7 @@
         <v>107920102</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1169,7 +1166,7 @@
         <v>108112488</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1201,7 +1198,7 @@
         <v>107609757</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1233,7 +1230,7 @@
         <v>10855887</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1265,7 +1262,7 @@
         <v>106994293</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1297,7 +1294,7 @@
         <v>106794913</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -1329,7 +1326,7 @@
         <v>107555486</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1361,7 +1358,7 @@
         <v>108557818</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1393,7 +1390,7 @@
         <v>106822692</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -1425,7 +1422,7 @@
         <v>106931496</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -1466,21 +1463,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G139"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1497,13 +1494,13 @@
         <v>7</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1526,7 +1523,7 @@
         <v>107528627</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1549,7 +1546,7 @@
         <v>107528627</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1572,7 +1569,7 @@
         <v>107528627</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1595,7 +1592,7 @@
         <v>107528627</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1618,7 +1615,7 @@
         <v>107528627</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1641,7 +1638,7 @@
         <v>107528627</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1664,7 +1661,7 @@
         <v>107512302</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1687,7 +1684,7 @@
         <v>107512302</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1710,7 +1707,7 @@
         <v>107512302</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1733,7 +1730,7 @@
         <v>107512302</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1756,7 +1753,7 @@
         <v>107512302</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1779,7 +1776,7 @@
         <v>107512302</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1802,7 +1799,7 @@
         <v>106824965</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1825,7 +1822,7 @@
         <v>106824965</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1848,7 +1845,7 @@
         <v>106824965</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -1871,7 +1868,7 @@
         <v>106824965</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -1894,7 +1891,7 @@
         <v>106824965</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -1917,7 +1914,7 @@
         <v>106824965</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -1940,7 +1937,7 @@
         <v>1083514</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -1963,7 +1960,7 @@
         <v>1083514</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -1986,7 +1983,7 @@
         <v>1083514</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -2009,7 +2006,7 @@
         <v>1083514</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -2032,7 +2029,7 @@
         <v>1083514</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -2055,7 +2052,7 @@
         <v>1083514</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -2078,7 +2075,7 @@
         <v>1083514</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -2101,7 +2098,7 @@
         <v>107139542</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -2124,7 +2121,7 @@
         <v>107139542</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>13</v>
       </c>
@@ -2147,7 +2144,7 @@
         <v>107139542</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -2170,7 +2167,7 @@
         <v>107139542</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -2193,7 +2190,7 @@
         <v>107139542</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -2216,7 +2213,7 @@
         <v>108478858</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -2239,7 +2236,7 @@
         <v>108478858</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -2262,7 +2259,7 @@
         <v>108478858</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -2285,7 +2282,7 @@
         <v>108478858</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -2308,7 +2305,7 @@
         <v>108478858</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -2331,7 +2328,7 @@
         <v>108478858</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>15</v>
       </c>
@@ -2354,7 +2351,7 @@
         <v>107885592</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>15</v>
       </c>
@@ -2377,7 +2374,7 @@
         <v>107885592</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>15</v>
       </c>
@@ -2400,7 +2397,7 @@
         <v>107885592</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>15</v>
       </c>
@@ -2423,7 +2420,7 @@
         <v>107885592</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>15</v>
       </c>
@@ -2446,7 +2443,7 @@
         <v>107885592</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>15</v>
       </c>
@@ -2469,7 +2466,7 @@
         <v>107885592</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>16</v>
       </c>
@@ -2492,7 +2489,7 @@
         <v>108322903</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>16</v>
       </c>
@@ -2515,7 +2512,7 @@
         <v>108322903</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>16</v>
       </c>
@@ -2538,7 +2535,7 @@
         <v>108322903</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>16</v>
       </c>
@@ -2561,7 +2558,7 @@
         <v>108322903</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>16</v>
       </c>
@@ -2584,7 +2581,7 @@
         <v>108322903</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>16</v>
       </c>
@@ -2607,7 +2604,7 @@
         <v>108322903</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>17</v>
       </c>
@@ -2630,7 +2627,7 @@
         <v>10730529</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>17</v>
       </c>
@@ -2653,7 +2650,7 @@
         <v>10730529</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>17</v>
       </c>
@@ -2676,7 +2673,7 @@
         <v>10730529</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>17</v>
       </c>
@@ -2699,7 +2696,7 @@
         <v>10730529</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>17</v>
       </c>
@@ -2722,7 +2719,7 @@
         <v>10730529</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>17</v>
       </c>
@@ -2745,7 +2742,7 @@
         <v>10730529</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>18</v>
       </c>
@@ -2768,7 +2765,7 @@
         <v>108482982</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>18</v>
       </c>
@@ -2791,7 +2788,7 @@
         <v>108482982</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>18</v>
       </c>
@@ -2814,7 +2811,7 @@
         <v>108482982</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>18</v>
       </c>
@@ -2837,7 +2834,7 @@
         <v>108482982</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>18</v>
       </c>
@@ -2860,7 +2857,7 @@
         <v>108482982</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>18</v>
       </c>
@@ -2883,7 +2880,7 @@
         <v>108482982</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>19</v>
       </c>
@@ -2906,7 +2903,7 @@
         <v>108227876</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>19</v>
       </c>
@@ -2929,7 +2926,7 @@
         <v>108227876</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>19</v>
       </c>
@@ -2952,7 +2949,7 @@
         <v>108227876</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>19</v>
       </c>
@@ -2975,7 +2972,7 @@
         <v>108227876</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>19</v>
       </c>
@@ -2998,7 +2995,7 @@
         <v>108227876</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>19</v>
       </c>
@@ -3021,7 +3018,7 @@
         <v>108227876</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>20</v>
       </c>
@@ -3044,7 +3041,7 @@
         <v>108495155</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>20</v>
       </c>
@@ -3067,7 +3064,7 @@
         <v>108495155</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>20</v>
       </c>
@@ -3090,7 +3087,7 @@
         <v>108495155</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>20</v>
       </c>
@@ -3113,7 +3110,7 @@
         <v>108495155</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>20</v>
       </c>
@@ -3136,7 +3133,7 @@
         <v>108495155</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>20</v>
       </c>
@@ -3159,7 +3156,7 @@
         <v>108495155</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>21</v>
       </c>
@@ -3182,7 +3179,7 @@
         <v>107446541</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>21</v>
       </c>
@@ -3205,7 +3202,7 @@
         <v>107446541</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>21</v>
       </c>
@@ -3228,7 +3225,7 @@
         <v>107446541</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>21</v>
       </c>
@@ -3251,7 +3248,7 @@
         <v>107446541</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>21</v>
       </c>
@@ -3274,7 +3271,7 @@
         <v>107446541</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>21</v>
       </c>
@@ -3297,7 +3294,7 @@
         <v>107446541</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>22</v>
       </c>
@@ -3320,7 +3317,7 @@
         <v>107762495</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>22</v>
       </c>
@@ -3343,7 +3340,7 @@
         <v>107762495</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>22</v>
       </c>
@@ -3366,7 +3363,7 @@
         <v>107762495</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>22</v>
       </c>
@@ -3389,7 +3386,7 @@
         <v>107762495</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>22</v>
       </c>
@@ -3412,7 +3409,7 @@
         <v>107762495</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>22</v>
       </c>
@@ -3435,7 +3432,7 @@
         <v>107762495</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>24</v>
       </c>
@@ -3458,7 +3455,7 @@
         <v>107920102</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>24</v>
       </c>
@@ -3481,7 +3478,7 @@
         <v>107920102</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>24</v>
       </c>
@@ -3504,7 +3501,7 @@
         <v>107920102</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>24</v>
       </c>
@@ -3527,7 +3524,7 @@
         <v>107920102</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>24</v>
       </c>
@@ -3550,7 +3547,7 @@
         <v>107920102</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>24</v>
       </c>
@@ -3573,7 +3570,7 @@
         <v>107920102</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>25</v>
       </c>
@@ -3596,7 +3593,7 @@
         <v>108112488</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>25</v>
       </c>
@@ -3619,7 +3616,7 @@
         <v>108112488</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>25</v>
       </c>
@@ -3642,7 +3639,7 @@
         <v>108112488</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>25</v>
       </c>
@@ -3665,7 +3662,7 @@
         <v>108112488</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>25</v>
       </c>
@@ -3688,7 +3685,7 @@
         <v>108112488</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>25</v>
       </c>
@@ -3711,7 +3708,7 @@
         <v>108112488</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>27</v>
       </c>
@@ -3734,7 +3731,7 @@
         <v>10855887</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>27</v>
       </c>
@@ -3757,7 +3754,7 @@
         <v>10855887</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>27</v>
       </c>
@@ -3780,7 +3777,7 @@
         <v>10855887</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>27</v>
       </c>
@@ -3803,7 +3800,7 @@
         <v>10855887</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>27</v>
       </c>
@@ -3826,7 +3823,7 @@
         <v>10855887</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>27</v>
       </c>
@@ -3849,7 +3846,7 @@
         <v>10855887</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>28</v>
       </c>
@@ -3872,7 +3869,7 @@
         <v>106994293</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>28</v>
       </c>
@@ -3895,7 +3892,7 @@
         <v>106994293</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>28</v>
       </c>
@@ -3918,7 +3915,7 @@
         <v>106994293</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>28</v>
       </c>
@@ -3941,7 +3938,7 @@
         <v>106994293</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>28</v>
       </c>
@@ -3964,7 +3961,7 @@
         <v>106994293</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>28</v>
       </c>
@@ -3987,7 +3984,7 @@
         <v>106994293</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>29</v>
       </c>
@@ -4010,7 +4007,7 @@
         <v>106794913</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>29</v>
       </c>
@@ -4033,7 +4030,7 @@
         <v>106794913</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>29</v>
       </c>
@@ -4056,7 +4053,7 @@
         <v>106794913</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>29</v>
       </c>
@@ -4079,7 +4076,7 @@
         <v>106794913</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>29</v>
       </c>
@@ -4102,7 +4099,7 @@
         <v>106794913</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>29</v>
       </c>
@@ -4125,7 +4122,7 @@
         <v>106794913</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>30</v>
       </c>
@@ -4148,7 +4145,7 @@
         <v>107555486</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>30</v>
       </c>
@@ -4171,7 +4168,7 @@
         <v>107555486</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>30</v>
       </c>
@@ -4194,7 +4191,7 @@
         <v>107555486</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>30</v>
       </c>
@@ -4217,7 +4214,7 @@
         <v>107555486</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>30</v>
       </c>
@@ -4240,7 +4237,7 @@
         <v>107555486</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>30</v>
       </c>
@@ -4263,7 +4260,7 @@
         <v>107555486</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>31</v>
       </c>
@@ -4286,7 +4283,7 @@
         <v>108557818</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>31</v>
       </c>
@@ -4309,7 +4306,7 @@
         <v>108557818</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>31</v>
       </c>
@@ -4332,7 +4329,7 @@
         <v>108557818</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>31</v>
       </c>
@@ -4355,7 +4352,7 @@
         <v>108557818</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>31</v>
       </c>
@@ -4378,7 +4375,7 @@
         <v>108557818</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>31</v>
       </c>
@@ -4401,7 +4398,7 @@
         <v>108557818</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>33</v>
       </c>
@@ -4424,7 +4421,7 @@
         <v>106932576</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>33</v>
       </c>
@@ -4447,7 +4444,7 @@
         <v>106932576</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>33</v>
       </c>
@@ -4470,7 +4467,7 @@
         <v>106932576</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>33</v>
       </c>
@@ -4493,7 +4490,7 @@
         <v>106932576</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>33</v>
       </c>
@@ -4516,7 +4513,7 @@
         <v>106932576</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>33</v>
       </c>
@@ -4539,7 +4536,7 @@
         <v>106932576</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>34</v>
       </c>
@@ -4562,7 +4559,7 @@
         <v>1081971</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>34</v>
       </c>
@@ -4585,7 +4582,7 @@
         <v>1081971</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>34</v>
       </c>
@@ -4608,7 +4605,7 @@
         <v>1081971</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>34</v>
       </c>
@@ -4631,7 +4628,7 @@
         <v>1081971</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>34</v>
       </c>
@@ -4654,7 +4651,7 @@
         <v>1081971</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>34</v>
       </c>
@@ -4686,21 +4683,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4714,16 +4711,16 @@
         <v>37</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -4746,7 +4743,7 @@
         <v>107172509</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -4769,7 +4766,7 @@
         <v>107172509</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -4792,7 +4789,7 @@
         <v>107172509</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -4815,7 +4812,7 @@
         <v>107172509</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -4838,7 +4835,7 @@
         <v>107172509</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -4861,7 +4858,7 @@
         <v>107172509</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -4884,7 +4881,7 @@
         <v>106932576</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -4907,7 +4904,7 @@
         <v>106932576</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -4930,7 +4927,7 @@
         <v>106932576</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -4953,7 +4950,7 @@
         <v>106932576</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -4976,7 +4973,7 @@
         <v>106932576</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -4999,7 +4996,7 @@
         <v>106932576</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -5022,7 +5019,7 @@
         <v>107609757</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -5045,7 +5042,7 @@
         <v>107609757</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -5068,7 +5065,7 @@
         <v>107609757</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -5091,7 +5088,7 @@
         <v>107609757</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -5114,7 +5111,7 @@
         <v>107609757</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -5137,7 +5134,7 @@
         <v>107609757</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -5160,7 +5157,7 @@
         <v>106822692</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -5183,7 +5180,7 @@
         <v>106822692</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -5206,7 +5203,7 @@
         <v>106822692</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -5229,7 +5226,7 @@
         <v>106822692</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -5252,7 +5249,7 @@
         <v>106822692</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>32</v>
       </c>

</xml_diff>